<commit_message>
Inventory of GH 7
everything that is remaining post planting
</commit_message>
<xml_diff>
--- a/Planning/planning_2017/plotmaps_2017.xlsx
+++ b/Planning/planning_2017/plotmaps_2017.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="511" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="20760" tabRatio="511" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2 (2)" sheetId="6" r:id="rId1"/>
@@ -7356,7 +7356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -10297,7 +10297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -13216,7 +13216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView topLeftCell="B8" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="AD33" sqref="AD33"/>
     </sheetView>
   </sheetViews>
@@ -14693,7 +14693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
@@ -16144,7 +16144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -17554,7 +17554,7 @@
   </sheetPr>
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="AF21" sqref="AF21"/>
     </sheetView>
   </sheetViews>
@@ -19043,7 +19043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -20532,7 +20532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -22017,7 +22017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
@@ -24979,7 +24979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="AL23" sqref="AL23"/>
     </sheetView>
   </sheetViews>
@@ -26461,7 +26461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="B20" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>

</xml_diff>